<commit_message>
100 use cc koshi
</commit_message>
<xml_diff>
--- a/doc/completion/UseCaseConfiguration/100系_ユースケース構成.xlsx
+++ b/doc/completion/UseCaseConfiguration/100系_ユースケース構成.xlsx
@@ -10,12 +10,12 @@
     <sheet name="UC100ログイン" sheetId="1" r:id="rId1"/>
     <sheet name="UC102ログアウト" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
   <si>
     <t>画面ID</t>
     <rPh sb="0" eb="2">
@@ -230,13 +230,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>LoginView.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Menu.jsp</t>
-  </si>
-  <si>
     <t>ログイン画面</t>
     <rPh sb="4" eb="6">
       <t>ガメン</t>
@@ -245,16 +238,6 @@
   </si>
   <si>
     <t>新規登録</t>
-    <rPh sb="0" eb="2">
-      <t>シンキ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>トウロク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>新規登録</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -315,14 +298,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0100_01_03</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0100_01_02</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>M_01</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -352,37 +327,6 @@
   </si>
   <si>
     <t>HotelSearch.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>M_02</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>NewAccountView.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>OrderListView.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ShoppingcartView.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LogoutView.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Menu.jsp（ポップアップを表示）</t>
-    <rPh sb="16" eb="18">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Menu.jsp（ポップアップを表示）</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -397,10 +341,6 @@
     <rPh sb="12" eb="13">
       <t>オコナ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>NewAccountView.jsp</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -475,65 +415,129 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>メンバー名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カート</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>△</t>
+  </si>
+  <si>
+    <t>Menu.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>失敗</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Error.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M_01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TOPへ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>102_01</t>
+  </si>
+  <si>
+    <t>Logout.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログアウト画面</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Error.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メニューに戻る</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>　ヘッダー（ログイン時）</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>メンバー名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>カート</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>△</t>
-  </si>
-  <si>
-    <t>Menu.jsp</t>
+    <t>メインメニュー
+　ヘッダー（ログイン時）</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>成功</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Menu.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>失敗</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Error.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>M_01</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>TOPへ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>102_01</t>
+    <rPh sb="0" eb="2">
+      <t>セイコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アカウントをお持ちでない方はコチラ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログイン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0101_01_01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MainMenu.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MainMenu.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MainMenu.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MainMenu.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Login.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NewAccount.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OrderList.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Shoppingcart.jsp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NewAccount.jsp</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Logout.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ログアウト画面</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Error.jsp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メニューに戻る</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -619,7 +623,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -878,21 +882,6 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -932,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1045,19 +1034,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1076,6 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1084,27 +1074,55 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1134,43 +1152,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2405,10 +2386,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2433,20 +2414,20 @@
         <v>9</v>
       </c>
       <c r="B2" s="20"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="71"/>
+      <c r="D2" s="82"/>
       <c r="E2" s="29" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="71"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="25"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
@@ -2459,13 +2440,13 @@
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="23" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="27"/>
@@ -2480,55 +2461,55 @@
       <c r="A5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="87" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="79"/>
-      <c r="H6" s="72" t="s">
+      <c r="G6" s="90"/>
+      <c r="H6" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="80" t="s">
+      <c r="I6" s="84"/>
+      <c r="J6" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="80" t="s">
+      <c r="K6" s="76"/>
+      <c r="L6" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="82"/>
-      <c r="N6" s="81"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="76"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="75"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="86"/>
       <c r="J7" s="7" t="s">
         <v>12</v>
       </c>
@@ -2547,16 +2528,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
@@ -2565,7 +2546,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -2576,7 +2557,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="35"/>
       <c r="B9" s="35" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -2584,26 +2565,24 @@
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+        <v>56</v>
+      </c>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="35"/>
       <c r="B10" s="35"/>
       <c r="C10" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>46</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D10" s="34"/>
       <c r="E10" s="45"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
@@ -2611,13 +2590,13 @@
         <v>22</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="35"/>
@@ -2628,34 +2607,32 @@
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="35"/>
       <c r="B12" s="35"/>
       <c r="C12" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>45</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D12" s="34"/>
       <c r="E12" s="45"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="40" t="s">
-        <v>61</v>
+      <c r="I12" s="38" t="s">
+        <v>86</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -2672,27 +2649,27 @@
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
       <c r="H13" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="35"/>
       <c r="B14" s="35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="37"/>
@@ -2701,7 +2678,7 @@
         <v>22</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
@@ -2718,25 +2695,25 @@
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I15" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+        <v>57</v>
+      </c>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -2745,7 +2722,7 @@
         <v>22</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
@@ -2762,25 +2739,25 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+        <v>57</v>
+      </c>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
@@ -2789,7 +2766,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -2806,27 +2783,27 @@
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
       <c r="H19" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20" s="35"/>
       <c r="B20" s="35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="37"/>
@@ -2835,7 +2812,7 @@
         <v>22</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -2852,25 +2829,25 @@
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
       <c r="H21" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
+        <v>57</v>
+      </c>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E22" s="37"/>
       <c r="F22" s="37"/>
@@ -2879,7 +2856,7 @@
         <v>22</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -2896,25 +2873,25 @@
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
       <c r="H23" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24" s="35"/>
       <c r="B24" s="35"/>
       <c r="C24" s="10" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
@@ -2923,7 +2900,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="38" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
@@ -2940,25 +2917,25 @@
       <c r="F25" s="37"/>
       <c r="G25" s="37"/>
       <c r="H25" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="35"/>
       <c r="B26" s="35"/>
       <c r="C26" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
@@ -2967,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="I26" s="38" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="J26" s="41"/>
       <c r="K26" s="13"/>
@@ -2984,36 +2961,36 @@
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
       <c r="H27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A28" s="35"/>
       <c r="B28" s="35" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C28" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="62"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="65"/>
+        <v>71</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="66"/>
       <c r="H28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I28" s="40" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="I28" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -3025,37 +3002,37 @@
       <c r="A29" s="35"/>
       <c r="B29" s="35"/>
       <c r="C29" s="34"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="66"/>
       <c r="H29" s="5" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="I29" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="J29" s="59"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30" s="35"/>
       <c r="B30" s="35"/>
       <c r="C30" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="61"/>
+        <v>65</v>
+      </c>
+      <c r="D30" s="62"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="66"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="37"/>
       <c r="H30" s="5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I30" s="40" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -3070,40 +3047,40 @@
       <c r="D31" s="56"/>
       <c r="E31" s="57"/>
       <c r="F31" s="58"/>
-      <c r="G31" s="49"/>
+      <c r="G31" s="48"/>
       <c r="H31" s="42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
+        <v>69</v>
+      </c>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A32" s="83" t="s">
+      <c r="A32" s="78" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="87" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="85"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="85"/>
+        <v>27</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="63"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="66"/>
       <c r="H32" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="47" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
@@ -3112,101 +3089,107 @@
       <c r="N32" s="13"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A33" s="89"/>
+      <c r="A33" s="79"/>
       <c r="B33" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="92"/>
-      <c r="G33" s="91"/>
+        <v>88</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="66"/>
       <c r="H33" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+        <v>88</v>
+      </c>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+    </row>
+    <row r="34" spans="1:14" ht="27" x14ac:dyDescent="0.15">
       <c r="A34" s="35"/>
       <c r="B34" s="35"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="38"/>
-      <c r="J34" s="88"/>
-      <c r="K34" s="88"/>
-      <c r="L34" s="88"/>
-      <c r="M34" s="88"/>
-      <c r="N34" s="88"/>
+      <c r="C34" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="63"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="70"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="41"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A35" s="52"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="68"/>
+      <c r="A35" s="51"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="52"/>
       <c r="H35" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I35" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="88"/>
-      <c r="N35" s="88"/>
-    </row>
-    <row r="37" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="84" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="84"/>
-      <c r="F37" s="69"/>
+        <v>56</v>
+      </c>
+      <c r="J35" s="73"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="53"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="D37" s="15"/>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="M38" s="69"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="D39" s="15"/>
+      <c r="D39" s="16"/>
       <c r="E39" t="s">
-        <v>16</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="C40" s="69"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="D41" s="16"/>
+      <c r="D41" s="14"/>
       <c r="E41" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="D43" s="14"/>
-      <c r="E43" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="B44" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="80"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="12">
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="H6:I7"/>
@@ -3231,7 +3214,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3256,20 +3239,20 @@
         <v>9</v>
       </c>
       <c r="B2" s="20"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="71"/>
+      <c r="D2" s="82"/>
       <c r="E2" s="30" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="71"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="25"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
@@ -3282,13 +3265,13 @@
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="23" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="27"/>
@@ -3303,55 +3286,55 @@
       <c r="A5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="87" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="79"/>
-      <c r="H6" s="72" t="s">
+      <c r="G6" s="90"/>
+      <c r="H6" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="73"/>
-      <c r="J6" s="80" t="s">
+      <c r="I6" s="84"/>
+      <c r="J6" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="80" t="s">
+      <c r="K6" s="76"/>
+      <c r="L6" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="82"/>
-      <c r="N6" s="81"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="76"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="77"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
       <c r="F7" s="31" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="74"/>
-      <c r="I7" s="75"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="86"/>
       <c r="J7" s="7" t="s">
         <v>12</v>
       </c>
@@ -3368,18 +3351,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
@@ -3388,57 +3371,57 @@
         <v>22</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
+        <v>93</v>
+      </c>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52" t="s">
-        <v>36</v>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="52"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="68"/>
       <c r="F9" s="68"/>
       <c r="G9" s="68"/>
       <c r="H9" s="42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+        <v>55</v>
+      </c>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="62"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="65"/>
+        <v>76</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="66"/>
       <c r="H10" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -3447,20 +3430,20 @@
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="50"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="49"/>
       <c r="D11" s="56"/>
       <c r="E11" s="57"/>
       <c r="F11" s="58"/>
-      <c r="G11" s="49"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" s="51" t="s">
-        <v>90</v>
+        <v>68</v>
+      </c>
+      <c r="I11" s="50" t="s">
+        <v>75</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -3494,16 +3477,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="H6:I7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="H6:I7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>